<commit_message>
Update Pertanggal 17 Januari 2023 17:38 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_UserRole.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_UserRole.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Super User</t>
   </si>
@@ -101,6 +101,36 @@
   </si>
   <si>
     <t>SYS_PID</t>
+  </si>
+  <si>
+    <t>Project General Manager</t>
+  </si>
+  <si>
+    <t>Project Management Officer</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Site Manager</t>
+  </si>
+  <si>
+    <t>Project Controller Supervisor</t>
+  </si>
+  <si>
+    <t>Project Controller Staff</t>
+  </si>
+  <si>
+    <t>Project Administrator Supervisor</t>
+  </si>
+  <si>
+    <t>Project Administrator Staff</t>
+  </si>
+  <si>
+    <t>Project Worker Supervisor</t>
+  </si>
+  <si>
+    <t>Project Worker Staff</t>
   </si>
 </sst>
 </file>
@@ -474,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D35"/>
+  <dimension ref="B1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -521,7 +551,7 @@
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="str">
-        <f t="shared" ref="C4:C35" si="0">IF(EXACT(B4,""),"",CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_UserRole_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '",B4,"');"))</f>
+        <f t="shared" ref="C4:C46" si="0">IF(EXACT(B4,""),"",CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_UserRole_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '",B4,"');"))</f>
         <v/>
       </c>
       <c r="D4" s="5"/>
@@ -664,11 +694,11 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Finance, Accounting, &amp; Tax General Manager');</v>
+        <f t="shared" ref="C17" si="1">IF(EXACT(B17,""),"",CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_UserRole_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '",B17,"');"))</f>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project General Manager');</v>
       </c>
       <c r="D17" s="5">
         <v>95000000000013</v>
@@ -676,11 +706,11 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'HR, GA, &amp; TAM General Manager');</v>
+        <f t="shared" ref="C18" si="2">IF(EXACT(B18,""),"",CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_UserRole_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '",B18,"');"))</f>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project Management Officer');</v>
       </c>
       <c r="D18" s="5">
         <v>95000000000014</v>
@@ -688,55 +718,55 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Sales General Manager');</v>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Finance, Accounting, &amp; Tax General Manager');</v>
       </c>
       <c r="D19" s="5">
         <v>95000000000015</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D20" s="5"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'HR, GA, &amp; TAM General Manager');</v>
+      </c>
+      <c r="D20" s="5">
+        <v>95000000000016</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Finance Manager');</v>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Sales General Manager');</v>
       </c>
       <c r="D21" s="5">
-        <v>95000000000016</v>
+        <v>95000000000017</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Cashier &amp; Treasury Senior Staff');</v>
-      </c>
-      <c r="D22" s="5">
-        <v>95000000000017</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Cashier &amp; Treasury Staff');</v>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project Manager');</v>
       </c>
       <c r="D23" s="5">
         <v>95000000000018</v>
@@ -744,11 +774,11 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Cost Controller Senior Staff');</v>
+        <f t="shared" ref="C24:C31" si="3">IF(EXACT(B24,""),"",CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_UserRole_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '",B24,"');"))</f>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Site Manager');</v>
       </c>
       <c r="D24" s="5">
         <v>95000000000019</v>
@@ -756,126 +786,254 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Cost Controller Staff');</v>
+        <f t="shared" si="3"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project Controller Supervisor');</v>
       </c>
       <c r="D25" s="5">
         <v>95000000000020</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D26" s="5"/>
+        <f t="shared" ref="C26:C28" si="4">IF(EXACT(B26,""),"",CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_UserRole_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '",B26,"');"))</f>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project Controller Staff');</v>
+      </c>
+      <c r="D26" s="5">
+        <v>95000000000021</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Accounting &amp; Tax Manager');</v>
+        <f t="shared" si="4"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project Administrator Supervisor');</v>
       </c>
       <c r="D27" s="5">
-        <v>95000000000021</v>
+        <v>95000000000022</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Accounting &amp; Tax Senior Staff');</v>
+        <f t="shared" si="4"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project Administrator Staff');</v>
       </c>
       <c r="D28" s="5">
-        <v>95000000000022</v>
+        <v>95000000000023</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Accounting &amp; Tax Staff');</v>
+        <f t="shared" ref="C29:C30" si="5">IF(EXACT(B29,""),"",CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_UserRole_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '",B29,"');"))</f>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project Worker Supervisor');</v>
       </c>
       <c r="D29" s="5">
-        <v>95000000000023</v>
+        <v>95000000000024</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C30" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Project Worker Staff');</v>
+      </c>
+      <c r="D30" s="5">
+        <v>95000000000025</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="1" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT System Manager');</v>
-      </c>
-      <c r="D31" s="5">
-        <v>95000000000024</v>
-      </c>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT System Engineer Supervisor');</v>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Finance Manager');</v>
       </c>
       <c r="D32" s="5">
-        <v>95000000000025</v>
+        <v>95000000000026</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT System Engineer Staff');</v>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Cashier &amp; Treasury Senior Staff');</v>
       </c>
       <c r="D33" s="5">
-        <v>95000000000026</v>
+        <v>95000000000027</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT Software Engineer Supervisor');</v>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Cashier &amp; Treasury Staff');</v>
       </c>
       <c r="D34" s="5">
-        <v>95000000000027</v>
+        <v>95000000000028</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Cost Controller Senior Staff');</v>
+      </c>
+      <c r="D35" s="5">
+        <v>95000000000029</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Cost Controller Staff');</v>
+      </c>
+      <c r="D36" s="5">
+        <v>95000000000030</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="2"/>
+      <c r="C37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Accounting &amp; Tax Manager');</v>
+      </c>
+      <c r="D38" s="5">
+        <v>95000000000031</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Accounting &amp; Tax Senior Staff');</v>
+      </c>
+      <c r="D39" s="5">
+        <v>95000000000032</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Accounting &amp; Tax Staff');</v>
+      </c>
+      <c r="D40" s="5">
+        <v>95000000000033</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT System Manager');</v>
+      </c>
+      <c r="D42" s="5">
+        <v>95000000000034</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT System Engineer Supervisor');</v>
+      </c>
+      <c r="D43" s="5">
+        <v>95000000000035</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT System Engineer Staff');</v>
+      </c>
+      <c r="D44" s="5">
+        <v>95000000000036</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT Software Engineer Supervisor');</v>
+      </c>
+      <c r="D45" s="5">
+        <v>95000000000037</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="1" t="str">
+      <c r="C46" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'IT Software Engineer Staff');</v>
       </c>
-      <c r="D35" s="5">
-        <v>95000000000028</v>
+      <c r="D46" s="5">
+        <v>95000000000038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Pertanggal 15 November 2024 16:18 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_UserRole.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_UserRole.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Super User</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Human Resource Development Staff</t>
+  </si>
+  <si>
+    <t>Tools And Asset Manager</t>
+  </si>
+  <si>
+    <t>Tools And Asset Senior Staff</t>
+  </si>
+  <si>
+    <t>Tools And Asset Staff</t>
   </si>
 </sst>
 </file>
@@ -543,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D63"/>
+  <dimension ref="B1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1263,6 +1272,50 @@
         <v>95000000000051</v>
       </c>
     </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="2"/>
+      <c r="C64" s="1" t="str">
+        <f t="shared" ref="C64:C67" si="10">IF(EXACT(B64,""),"",CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_UserRole_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '",B64,"');"))</f>
+        <v/>
+      </c>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C65" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Tools And Asset Manager');</v>
+      </c>
+      <c r="D65" s="5">
+        <v>95000000000052</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Tools And Asset Senior Staff');</v>
+      </c>
+      <c r="D66" s="5">
+        <v>95000000000053</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_UserRole_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Tools And Asset Staff');</v>
+      </c>
+      <c r="D67" s="5">
+        <v>95000000000054</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>